<commit_message>
update break points for index and remove black from colour scale
</commit_message>
<xml_diff>
--- a/output/download-data/iTRAQI - ASGS 2021 SA2.xlsx
+++ b/output/download-data/iTRAQI - ASGS 2021 SA2.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1123" uniqueCount="592">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1123" uniqueCount="588">
   <si>
     <t>Suggested citation</t>
   </si>
@@ -1772,39 +1772,21 @@
     <t>2A</t>
   </si>
   <si>
-    <t>2B</t>
-  </si>
-  <si>
     <t>1A</t>
   </si>
   <si>
-    <t>4D</t>
-  </si>
-  <si>
     <t>4C</t>
   </si>
   <si>
+    <t>4B</t>
+  </si>
+  <si>
+    <t>3B</t>
+  </si>
+  <si>
     <t>3C</t>
   </si>
   <si>
-    <t>3D</t>
-  </si>
-  <si>
-    <t>4E</t>
-  </si>
-  <si>
-    <t>4B</t>
-  </si>
-  <si>
-    <t>3B</t>
-  </si>
-  <si>
-    <t>5E</t>
-  </si>
-  <si>
-    <t>5D</t>
-  </si>
-  <si>
     <t>4A</t>
   </si>
   <si>
@@ -1812,6 +1794,12 @@
   </si>
   <si>
     <t>5C</t>
+  </si>
+  <si>
+    <t>6C</t>
+  </si>
+  <si>
+    <t>5B</t>
   </si>
 </sst>
 </file>
@@ -3008,7 +2996,7 @@
         <v>101.5726379217939</v>
       </c>
       <c r="H14" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="15">
@@ -3034,7 +3022,7 @@
         <v>78.69149007856845</v>
       </c>
       <c r="H15" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="16">
@@ -3138,7 +3126,7 @@
         <v>22.56369379176067</v>
       </c>
       <c r="H19" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="20">
@@ -3268,7 +3256,7 @@
         <v>31.50493797655804</v>
       </c>
       <c r="H24" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="25">
@@ -3294,7 +3282,7 @@
         <v>23.29279001965665</v>
       </c>
       <c r="H25" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="26">
@@ -3320,7 +3308,7 @@
         <v>22.638505336687786</v>
       </c>
       <c r="H26" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="27">
@@ -3346,7 +3334,7 @@
         <v>16.403820073213183</v>
       </c>
       <c r="H27" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="28">
@@ -3372,7 +3360,7 @@
         <v>18.467925530030698</v>
       </c>
       <c r="H28" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="29">
@@ -3398,7 +3386,7 @@
         <v>20.061193715624086</v>
       </c>
       <c r="H29" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="30">
@@ -3424,7 +3412,7 @@
         <v>16.950567089892957</v>
       </c>
       <c r="H30" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="31">
@@ -3450,7 +3438,7 @@
         <v>16.863882672041655</v>
       </c>
       <c r="H31" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="32">
@@ -3476,7 +3464,7 @@
         <v>19.723977578209087</v>
       </c>
       <c r="H32" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="33">
@@ -3502,7 +3490,7 @@
         <v>14.102813809664212</v>
       </c>
       <c r="H33" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="34">
@@ -3528,7 +3516,7 @@
         <v>13.451062095334578</v>
       </c>
       <c r="H34" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="35">
@@ -3554,7 +3542,7 @@
         <v>14.951558730172792</v>
       </c>
       <c r="H35" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="36">
@@ -3580,7 +3568,7 @@
         <v>17.429150272497054</v>
       </c>
       <c r="H36" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="37">
@@ -3606,7 +3594,7 @@
         <v>26.46368633520501</v>
       </c>
       <c r="H37" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="38">
@@ -3658,7 +3646,7 @@
         <v>21.714653025353755</v>
       </c>
       <c r="H39" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="40">
@@ -3684,7 +3672,7 @@
         <v>20.507850058470467</v>
       </c>
       <c r="H40" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="41">
@@ -3710,7 +3698,7 @@
         <v>28.053008449603794</v>
       </c>
       <c r="H41" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="42">
@@ -3736,7 +3724,7 @@
         <v>16.926367884259776</v>
       </c>
       <c r="H42" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="43">
@@ -3762,7 +3750,7 @@
         <v>27.726890259245693</v>
       </c>
       <c r="H43" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="44">
@@ -3866,7 +3854,7 @@
         <v>24.449295775822293</v>
       </c>
       <c r="H47" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="48">
@@ -3892,7 +3880,7 @@
         <v>21.82165997509901</v>
       </c>
       <c r="H48" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="49">
@@ -3918,7 +3906,7 @@
         <v>14.901456405714953</v>
       </c>
       <c r="H49" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="50">
@@ -3944,7 +3932,7 @@
         <v>17.747680556759178</v>
       </c>
       <c r="H50" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="51">
@@ -3970,7 +3958,7 @@
         <v>18.918969474567803</v>
       </c>
       <c r="H51" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="52">
@@ -3996,7 +3984,7 @@
         <v>16.656664776227444</v>
       </c>
       <c r="H52" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="53">
@@ -4022,7 +4010,7 @@
         <v>19.87112842562692</v>
       </c>
       <c r="H53" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="54">
@@ -4048,7 +4036,7 @@
         <v>13.17794321158749</v>
       </c>
       <c r="H54" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="55">
@@ -4074,7 +4062,7 @@
         <v>14.527225865720425</v>
       </c>
       <c r="H55" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="56">
@@ -4100,7 +4088,7 @@
         <v>12.040621896017</v>
       </c>
       <c r="H56" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="57">
@@ -4126,7 +4114,7 @@
         <v>13.078403607890777</v>
       </c>
       <c r="H57" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="58">
@@ -4152,7 +4140,7 @@
         <v>15.845551128518878</v>
       </c>
       <c r="H58" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="59">
@@ -4178,7 +4166,7 @@
         <v>15.367198695853403</v>
       </c>
       <c r="H59" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="60">
@@ -4204,7 +4192,7 @@
         <v>11.23647665916576</v>
       </c>
       <c r="H60" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="61">
@@ -4230,7 +4218,7 @@
         <v>14.116259701848094</v>
       </c>
       <c r="H61" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="62">
@@ -4282,7 +4270,7 @@
         <v>19.065318488179855</v>
       </c>
       <c r="H63" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="64">
@@ -4308,7 +4296,7 @@
         <v>19.485849154141533</v>
       </c>
       <c r="H64" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="65">
@@ -4334,7 +4322,7 @@
         <v>17.633400162779935</v>
       </c>
       <c r="H65" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="66">
@@ -4386,7 +4374,7 @@
         <v>18.935739580684185</v>
       </c>
       <c r="H67" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="68">
@@ -4412,7 +4400,7 @@
         <v>19.984830256343457</v>
       </c>
       <c r="H68" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="69">
@@ -4438,7 +4426,7 @@
         <v>17.950475570276012</v>
       </c>
       <c r="H69" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="70">
@@ -4464,7 +4452,7 @@
         <v>15.058642005205797</v>
       </c>
       <c r="H70" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="71">
@@ -4490,7 +4478,7 @@
         <v>18.135901828091505</v>
       </c>
       <c r="H71" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="72">
@@ -4516,7 +4504,7 @@
         <v>17.295814638092338</v>
       </c>
       <c r="H72" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="73">
@@ -4542,7 +4530,7 @@
         <v>15.052779949709702</v>
       </c>
       <c r="H73" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="74">
@@ -4568,7 +4556,7 @@
         <v>22.6967797059516</v>
       </c>
       <c r="H74" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="75">
@@ -4672,7 +4660,7 @@
         <v>19.82528792858784</v>
       </c>
       <c r="H78" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="79">
@@ -4750,7 +4738,7 @@
         <v>19.61002144486463</v>
       </c>
       <c r="H81" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="82">
@@ -4776,7 +4764,7 @@
         <v>21.689806419069555</v>
       </c>
       <c r="H82" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="83">
@@ -4802,7 +4790,7 @@
         <v>19.79494611358541</v>
       </c>
       <c r="H83" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="84">
@@ -4828,7 +4816,7 @@
         <v>20.45010256813066</v>
       </c>
       <c r="H84" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="85">
@@ -4854,7 +4842,7 @@
         <v>21.864459430813213</v>
       </c>
       <c r="H85" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="86">
@@ -4880,7 +4868,7 @@
         <v>18.69196745982265</v>
       </c>
       <c r="H86" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="87">
@@ -4906,7 +4894,7 @@
         <v>20.92187674739148</v>
       </c>
       <c r="H87" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="88">
@@ -4958,7 +4946,7 @@
         <v>30.784904499279264</v>
       </c>
       <c r="H89" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="90">
@@ -4984,7 +4972,7 @@
         <v>16.321209649099956</v>
       </c>
       <c r="H90" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="91">
@@ -5010,7 +4998,7 @@
         <v>16.31320416529013</v>
       </c>
       <c r="H91" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="92">
@@ -5036,7 +5024,7 @@
         <v>18.185179680103374</v>
       </c>
       <c r="H92" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="93">
@@ -5088,7 +5076,7 @@
         <v>14.606738134029456</v>
       </c>
       <c r="H94" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="95">
@@ -5114,7 +5102,7 @@
         <v>16.406390455550763</v>
       </c>
       <c r="H95" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="96">
@@ -5140,7 +5128,7 @@
         <v>15.242187747564799</v>
       </c>
       <c r="H96" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="97">
@@ -5166,7 +5154,7 @@
         <v>15.454985100194563</v>
       </c>
       <c r="H97" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="98">
@@ -5192,7 +5180,7 @@
         <v>11.877757574552447</v>
       </c>
       <c r="H98" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="99">
@@ -5218,7 +5206,7 @@
         <v>13.168680521934675</v>
       </c>
       <c r="H99" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="100">
@@ -5244,7 +5232,7 @@
         <v>15.258867086336977</v>
       </c>
       <c r="H100" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="101">
@@ -5296,7 +5284,7 @@
         <v>17.845184738996977</v>
       </c>
       <c r="H102" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="103">
@@ -5322,7 +5310,7 @@
         <v>16.150631304970148</v>
       </c>
       <c r="H103" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="104">
@@ -5348,7 +5336,7 @@
         <v>18.011633096820788</v>
       </c>
       <c r="H104" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="105">
@@ -5374,7 +5362,7 @@
         <v>18.304227190032407</v>
       </c>
       <c r="H105" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="106">
@@ -5400,7 +5388,7 @@
         <v>22.71453717874067</v>
       </c>
       <c r="H106" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="107">
@@ -5426,7 +5414,7 @@
         <v>8.79468131837757</v>
       </c>
       <c r="H107" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="108">
@@ -5452,7 +5440,7 @@
         <v>7.3620774798539514</v>
       </c>
       <c r="H108" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="109">
@@ -5478,7 +5466,7 @@
         <v>10.214759140721867</v>
       </c>
       <c r="H109" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="110">
@@ -5504,7 +5492,7 @@
         <v>9.81868198568975</v>
       </c>
       <c r="H110" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="111">
@@ -5530,7 +5518,7 @@
         <v>9.499820195561824</v>
       </c>
       <c r="H111" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="112">
@@ -5556,7 +5544,7 @@
         <v>9.766936377797151</v>
       </c>
       <c r="H112" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="113">
@@ -5582,7 +5570,7 @@
         <v>7.269974757483169</v>
       </c>
       <c r="H113" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="114">
@@ -5608,7 +5596,7 @@
         <v>10.65169574913159</v>
       </c>
       <c r="H114" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="115">
@@ -5634,7 +5622,7 @@
         <v>12.36510621915204</v>
       </c>
       <c r="H115" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="116">
@@ -5660,7 +5648,7 @@
         <v>11.420120207621835</v>
       </c>
       <c r="H116" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="117">
@@ -5686,7 +5674,7 @@
         <v>10.89068940235154</v>
       </c>
       <c r="H117" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="118">
@@ -5712,7 +5700,7 @@
         <v>10.821280283632973</v>
       </c>
       <c r="H118" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="119">
@@ -5738,7 +5726,7 @@
         <v>14.091753618475877</v>
       </c>
       <c r="H119" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="120">
@@ -5764,7 +5752,7 @@
         <v>13.020281115957232</v>
       </c>
       <c r="H120" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="121">
@@ -5790,7 +5778,7 @@
         <v>10.159228689791007</v>
       </c>
       <c r="H121" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="122">
@@ -5816,7 +5804,7 @@
         <v>11.234165472211089</v>
       </c>
       <c r="H122" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="123">
@@ -5842,7 +5830,7 @@
         <v>14.162391615950696</v>
       </c>
       <c r="H123" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="124">
@@ -5868,7 +5856,7 @@
         <v>13.790803821465715</v>
       </c>
       <c r="H124" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="125">
@@ -5894,7 +5882,7 @@
         <v>10.680664604016783</v>
       </c>
       <c r="H125" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="126">
@@ -5920,7 +5908,7 @@
         <v>13.670607998489459</v>
       </c>
       <c r="H126" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="127">
@@ -5946,7 +5934,7 @@
         <v>15.526711532380887</v>
       </c>
       <c r="H127" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="128">
@@ -5972,7 +5960,7 @@
         <v>7.850103400339776</v>
       </c>
       <c r="H128" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="129">
@@ -5998,7 +5986,7 @@
         <v>9.443131338948433</v>
       </c>
       <c r="H129" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="130">
@@ -6024,7 +6012,7 @@
         <v>8.90033185572156</v>
       </c>
       <c r="H130" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="131">
@@ -6050,7 +6038,7 @@
         <v>8.221793170261662</v>
       </c>
       <c r="H131" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="132">
@@ -6076,7 +6064,7 @@
         <v>8.792744132514485</v>
       </c>
       <c r="H132" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="133">
@@ -6102,7 +6090,7 @@
         <v>13.09851045395635</v>
       </c>
       <c r="H133" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="134">
@@ -6128,7 +6116,7 @@
         <v>13.08618991004937</v>
       </c>
       <c r="H134" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="135">
@@ -6154,7 +6142,7 @@
         <v>10.431413313242047</v>
       </c>
       <c r="H135" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="136">
@@ -6180,7 +6168,7 @@
         <v>12.270481238030243</v>
       </c>
       <c r="H136" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="137">
@@ -6206,7 +6194,7 @@
         <v>10.065576104850606</v>
       </c>
       <c r="H137" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="138">
@@ -6232,7 +6220,7 @@
         <v>9.585157285321202</v>
       </c>
       <c r="H138" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="139">
@@ -6258,7 +6246,7 @@
         <v>12.58082692026619</v>
       </c>
       <c r="H139" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="140">
@@ -6284,7 +6272,7 @@
         <v>247.04863805255252</v>
       </c>
       <c r="H140" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="141">
@@ -6310,7 +6298,7 @@
         <v>274.0353472584943</v>
       </c>
       <c r="H141" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="142">
@@ -6336,7 +6324,7 @@
         <v>247.7683177483034</v>
       </c>
       <c r="H142" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="143">
@@ -6362,7 +6350,7 @@
         <v>259.6184048891374</v>
       </c>
       <c r="H143" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="144">
@@ -6388,7 +6376,7 @@
         <v>261.20329307714155</v>
       </c>
       <c r="H144" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="145">
@@ -6414,7 +6402,7 @@
         <v>255.81942416918048</v>
       </c>
       <c r="H145" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="146">
@@ -6440,7 +6428,7 @@
         <v>237.8036561129867</v>
       </c>
       <c r="H146" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="147">
@@ -6466,7 +6454,7 @@
         <v>243.80620385705038</v>
       </c>
       <c r="H147" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="148">
@@ -6492,7 +6480,7 @@
         <v>241.51222625503863</v>
       </c>
       <c r="H148" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="149">
@@ -6518,7 +6506,7 @@
         <v>236.25532102910768</v>
       </c>
       <c r="H149" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="150">
@@ -6544,7 +6532,7 @@
         <v>248.68534965436834</v>
       </c>
       <c r="H150" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="151">
@@ -6570,7 +6558,7 @@
         <v>244.63662826196207</v>
       </c>
       <c r="H151" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="152">
@@ -6596,7 +6584,7 @@
         <v>249.74520483995093</v>
       </c>
       <c r="H152" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="153">
@@ -6622,7 +6610,7 @@
         <v>243.3958949850894</v>
       </c>
       <c r="H153" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="154">
@@ -6648,7 +6636,7 @@
         <v>242.9708771063166</v>
       </c>
       <c r="H154" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="155">
@@ -6674,7 +6662,7 @@
         <v>237.4984010524355</v>
       </c>
       <c r="H155" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="156">
@@ -6700,7 +6688,7 @@
         <v>240.4025474616194</v>
       </c>
       <c r="H156" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="157">
@@ -6726,7 +6714,7 @@
         <v>236.99620298984712</v>
       </c>
       <c r="H157" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="158">
@@ -6752,7 +6740,7 @@
         <v>245.48914605311654</v>
       </c>
       <c r="H158" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="159">
@@ -6778,7 +6766,7 @@
         <v>239.56367543904605</v>
       </c>
       <c r="H159" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="160">
@@ -6804,7 +6792,7 @@
         <v>222.77203913159383</v>
       </c>
       <c r="H160" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="161">
@@ -6830,7 +6818,7 @@
         <v>183.08376098715917</v>
       </c>
       <c r="H161" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="162">
@@ -6856,7 +6844,7 @@
         <v>196.890974660668</v>
       </c>
       <c r="H162" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="163">
@@ -6882,7 +6870,7 @@
         <v>197.66924029958045</v>
       </c>
       <c r="H163" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="164">
@@ -6908,7 +6896,7 @@
         <v>221.67278362076718</v>
       </c>
       <c r="H164" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="165">
@@ -6934,7 +6922,7 @@
         <v>249.24260809993427</v>
       </c>
       <c r="H165" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="166">
@@ -6960,7 +6948,7 @@
         <v>394.42765559396014</v>
       </c>
       <c r="H166" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="167">
@@ -6986,7 +6974,7 @@
         <v>299.5003718201152</v>
       </c>
       <c r="H167" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="168">
@@ -7012,7 +7000,7 @@
         <v>261.65397270860444</v>
       </c>
       <c r="H168" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="169">
@@ -7038,7 +7026,7 @@
         <v>274.22713911344135</v>
       </c>
       <c r="H169" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="170">
@@ -7064,7 +7052,7 @@
         <v>282.88661718642857</v>
       </c>
       <c r="H170" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="171">
@@ -7090,7 +7078,7 @@
         <v>251.98484924073387</v>
       </c>
       <c r="H171" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="172">
@@ -7116,7 +7104,7 @@
         <v>275.9077777104578</v>
       </c>
       <c r="H172" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="173">
@@ -7142,7 +7130,7 @@
         <v>457.0307861583133</v>
       </c>
       <c r="H173" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
     </row>
     <row r="174">
@@ -7168,7 +7156,7 @@
         <v>271.90309629303067</v>
       </c>
       <c r="H174" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="175">
@@ -7194,7 +7182,7 @@
         <v>229.01430805189545</v>
       </c>
       <c r="H175" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="176">
@@ -7220,7 +7208,7 @@
         <v>336.8445743152373</v>
       </c>
       <c r="H176" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="177">
@@ -7246,7 +7234,7 @@
         <v>333.66196009826126</v>
       </c>
       <c r="H177" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="178">
@@ -7272,7 +7260,7 @@
         <v>322.2004947686238</v>
       </c>
       <c r="H178" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="179">
@@ -7298,7 +7286,7 @@
         <v>476.6378418189835</v>
       </c>
       <c r="H179" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
     </row>
     <row r="180">
@@ -7324,7 +7312,7 @@
         <v>272.3229400135193</v>
       </c>
       <c r="H180" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="181">
@@ -7350,7 +7338,7 @@
         <v>145.9553839159654</v>
       </c>
       <c r="H181" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="182">
@@ -7376,7 +7364,7 @@
         <v>146.72159800501208</v>
       </c>
       <c r="H182" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="183">
@@ -7402,7 +7390,7 @@
         <v>181.66704674202924</v>
       </c>
       <c r="H183" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="184">
@@ -7428,7 +7416,7 @@
         <v>131.14954160755815</v>
       </c>
       <c r="H184" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="185">
@@ -7454,7 +7442,7 @@
         <v>184.36669775358678</v>
       </c>
       <c r="H185" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="186">
@@ -7480,7 +7468,7 @@
         <v>126.50758055115159</v>
       </c>
       <c r="H186" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="187">
@@ -7506,7 +7494,7 @@
         <v>135.6600796888107</v>
       </c>
       <c r="H187" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="188">
@@ -7532,7 +7520,7 @@
         <v>146.91593905748857</v>
       </c>
       <c r="H188" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="189">
@@ -7558,7 +7546,7 @@
         <v>155.3190771075822</v>
       </c>
       <c r="H189" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="190">
@@ -7584,7 +7572,7 @@
         <v>202.65582018448492</v>
       </c>
       <c r="H190" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="191">
@@ -7610,7 +7598,7 @@
         <v>126.22656383978938</v>
       </c>
       <c r="H191" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="192">
@@ -7636,7 +7624,7 @@
         <v>489.77312546156816</v>
       </c>
       <c r="H192" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="193">
@@ -7662,7 +7650,7 @@
         <v>568.0258595958749</v>
       </c>
       <c r="H193" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="194">
@@ -7688,7 +7676,7 @@
         <v>487.2976278132609</v>
       </c>
       <c r="H194" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="195">
@@ -7714,7 +7702,7 @@
         <v>397.06620886656015</v>
       </c>
       <c r="H195" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="196">
@@ -7740,7 +7728,7 @@
         <v>404.15024553794774</v>
       </c>
       <c r="H196" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="197">
@@ -7766,7 +7754,7 @@
         <v>425.3756300152586</v>
       </c>
       <c r="H197" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="198">
@@ -7792,7 +7780,7 @@
         <v>406.4241808059397</v>
       </c>
       <c r="H198" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="199">
@@ -7818,7 +7806,7 @@
         <v>417.1073022907452</v>
       </c>
       <c r="H199" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="200">
@@ -7844,7 +7832,7 @@
         <v>401.9856445670707</v>
       </c>
       <c r="H200" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="201">
@@ -7870,7 +7858,7 @@
         <v>400.2766860151818</v>
       </c>
       <c r="H201" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="202">
@@ -7896,7 +7884,7 @@
         <v>410.73506331708325</v>
       </c>
       <c r="H202" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="203">
@@ -7922,7 +7910,7 @@
         <v>410.8739402682638</v>
       </c>
       <c r="H203" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="204">
@@ -7948,7 +7936,7 @@
         <v>397.9841099427009</v>
       </c>
       <c r="H204" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="205">
@@ -7974,7 +7962,7 @@
         <v>407.0910924298148</v>
       </c>
       <c r="H205" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="206">
@@ -8000,7 +7988,7 @@
         <v>394.1604949428149</v>
       </c>
       <c r="H206" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="207">
@@ -8026,7 +8014,7 @@
         <v>395.0341606328079</v>
       </c>
       <c r="H207" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="208">
@@ -8052,7 +8040,7 @@
         <v>425.29695853604403</v>
       </c>
       <c r="H208" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="209">
@@ -8078,7 +8066,7 @@
         <v>445.4327354044974</v>
       </c>
       <c r="H209" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="210">
@@ -8104,7 +8092,7 @@
         <v>445.1890621644038</v>
       </c>
       <c r="H210" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="211">
@@ -8130,7 +8118,7 @@
         <v>444.01763271334164</v>
       </c>
       <c r="H211" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="212">
@@ -8156,7 +8144,7 @@
         <v>391.7717629283861</v>
       </c>
       <c r="H212" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="213">
@@ -8182,7 +8170,7 @@
         <v>428.7984201950769</v>
       </c>
       <c r="H213" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="214">
@@ -8208,7 +8196,7 @@
         <v>436.6748760782118</v>
       </c>
       <c r="H214" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="215">
@@ -8234,7 +8222,7 @@
         <v>362.38358596808246</v>
       </c>
       <c r="H215" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="216">
@@ -8260,7 +8248,7 @@
         <v>311.9480900140645</v>
       </c>
       <c r="H216" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="217">
@@ -8286,7 +8274,7 @@
         <v>324.0932618598847</v>
       </c>
       <c r="H217" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="218">
@@ -8312,7 +8300,7 @@
         <v>336.74604118808065</v>
       </c>
       <c r="H218" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="219">
@@ -8338,7 +8326,7 @@
         <v>331.15085823789025</v>
       </c>
       <c r="H219" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="220">
@@ -8364,7 +8352,7 @@
         <v>330.9280614310575</v>
       </c>
       <c r="H220" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="221">
@@ -8390,7 +8378,7 @@
         <v>386.42651550012783</v>
       </c>
       <c r="H221" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="222">
@@ -8416,7 +8404,7 @@
         <v>327.6060143185889</v>
       </c>
       <c r="H222" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="223">
@@ -8442,7 +8430,7 @@
         <v>327.6713686330203</v>
       </c>
       <c r="H223" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="224">
@@ -8468,7 +8456,7 @@
         <v>326.5632988277705</v>
       </c>
       <c r="H224" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="225">
@@ -8494,7 +8482,7 @@
         <v>330.11660961031566</v>
       </c>
       <c r="H225" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="226">
@@ -8806,7 +8794,7 @@
         <v>14.89302853648337</v>
       </c>
       <c r="H237" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="238">
@@ -8884,7 +8872,7 @@
         <v>14.877243318360115</v>
       </c>
       <c r="H240" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="241">
@@ -9170,7 +9158,7 @@
         <v>16.09582258802459</v>
       </c>
       <c r="H251" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="252">
@@ -9248,7 +9236,7 @@
         <v>17.82975914547933</v>
       </c>
       <c r="H254" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="255">
@@ -9326,7 +9314,7 @@
         <v>20.197559757050158</v>
       </c>
       <c r="H257" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="258">
@@ -9664,7 +9652,7 @@
         <v>14.761115028043037</v>
       </c>
       <c r="H270" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="271">
@@ -9690,7 +9678,7 @@
         <v>14.664376224815896</v>
       </c>
       <c r="H271" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="272">
@@ -9716,7 +9704,7 @@
         <v>14.103160153940053</v>
       </c>
       <c r="H272" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="273">
@@ -9742,7 +9730,7 @@
         <v>13.404732443809735</v>
       </c>
       <c r="H273" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="274">
@@ -9768,7 +9756,7 @@
         <v>12.485830843094163</v>
       </c>
       <c r="H274" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="275">
@@ -9794,7 +9782,7 @@
         <v>14.846035457070116</v>
       </c>
       <c r="H275" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="276">
@@ -9846,7 +9834,7 @@
         <v>15.7445978337297</v>
       </c>
       <c r="H277" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="278">
@@ -9872,7 +9860,7 @@
         <v>12.299886246786059</v>
       </c>
       <c r="H278" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="279">
@@ -9924,7 +9912,7 @@
         <v>20.14026147714685</v>
       </c>
       <c r="H280" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="281">
@@ -9950,7 +9938,7 @@
         <v>20.625206385447655</v>
       </c>
       <c r="H281" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="282">
@@ -9976,7 +9964,7 @@
         <v>21.632642066756603</v>
       </c>
       <c r="H282" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="283">
@@ -10002,7 +9990,7 @@
         <v>18.67687863042329</v>
       </c>
       <c r="H283" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="284">
@@ -10028,7 +10016,7 @@
         <v>23.660650258030728</v>
       </c>
       <c r="H284" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="285">
@@ -10054,7 +10042,7 @@
         <v>22.518186627173236</v>
       </c>
       <c r="H285" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="286">
@@ -10080,7 +10068,7 @@
         <v>23.86689225370526</v>
       </c>
       <c r="H286" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="287">
@@ -10106,7 +10094,7 @@
         <v>103.2916452310468</v>
       </c>
       <c r="H287" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="288">
@@ -10132,7 +10120,7 @@
         <v>103.47160379110244</v>
       </c>
       <c r="H288" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="289">
@@ -10184,7 +10172,7 @@
         <v>76.08385538418418</v>
       </c>
       <c r="H290" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="291">
@@ -10860,7 +10848,7 @@
         <v>96.06849167195901</v>
       </c>
       <c r="H316" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="317">
@@ -11770,7 +11758,7 @@
         <v>142.61793784347117</v>
       </c>
       <c r="H351" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="352">
@@ -11796,7 +11784,7 @@
         <v>489.07592740836463</v>
       </c>
       <c r="H352" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="353">
@@ -11822,7 +11810,7 @@
         <v>519.2881299747824</v>
       </c>
       <c r="H353" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
     </row>
     <row r="354">
@@ -11848,7 +11836,7 @@
         <v>296.20450861260485</v>
       </c>
       <c r="H354" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="355">
@@ -11874,7 +11862,7 @@
         <v>357.53513239373365</v>
       </c>
       <c r="H355" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="356">
@@ -11900,7 +11888,7 @@
         <v>261.98477096805595</v>
       </c>
       <c r="H356" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="357">
@@ -11926,7 +11914,7 @@
         <v>268.33150011667055</v>
       </c>
       <c r="H357" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="358">
@@ -11952,7 +11940,7 @@
         <v>261.79191910839654</v>
       </c>
       <c r="H358" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="359">
@@ -11978,7 +11966,7 @@
         <v>270.9349385744697</v>
       </c>
       <c r="H359" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="360">
@@ -12004,7 +11992,7 @@
         <v>259.67460359318954</v>
       </c>
       <c r="H360" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="361">
@@ -12030,7 +12018,7 @@
         <v>263.6207876625067</v>
       </c>
       <c r="H361" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="362">
@@ -12056,7 +12044,7 @@
         <v>256.40706321956986</v>
       </c>
       <c r="H362" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="363">
@@ -12082,7 +12070,7 @@
         <v>260.90748423704906</v>
       </c>
       <c r="H363" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="364">
@@ -12108,7 +12096,7 @@
         <v>262.57237679585626</v>
       </c>
       <c r="H364" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="365">
@@ -12134,7 +12122,7 @@
         <v>269.61879963288914</v>
       </c>
       <c r="H365" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
     </row>
     <row r="366">
@@ -12160,7 +12148,7 @@
         <v>313.24568914081306</v>
       </c>
       <c r="H366" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
     </row>
     <row r="367">
@@ -12186,7 +12174,7 @@
         <v>305.1352292128772</v>
       </c>
       <c r="H367" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="368">
@@ -12212,7 +12200,7 @@
         <v>259.4858350959116</v>
       </c>
       <c r="H368" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="369">
@@ -12238,7 +12226,7 @@
         <v>263.84293394624126</v>
       </c>
       <c r="H369" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="370">
@@ -12264,7 +12252,7 @@
         <v>260.4635883927316</v>
       </c>
       <c r="H370" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="371">
@@ -12290,7 +12278,7 @@
         <v>271.35282835130204</v>
       </c>
       <c r="H371" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
     </row>
     <row r="372">
@@ -12316,7 +12304,7 @@
         <v>257.4801513691838</v>
       </c>
       <c r="H372" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="373">
@@ -12342,7 +12330,7 @@
         <v>246.81571863830743</v>
       </c>
       <c r="H373" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="374">
@@ -12368,7 +12356,7 @@
         <v>225.52371408865463</v>
       </c>
       <c r="H374" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="375">
@@ -12394,7 +12382,7 @@
         <v>199.1844127932079</v>
       </c>
       <c r="H375" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="376">
@@ -12654,7 +12642,7 @@
         <v>129.260916582017</v>
       </c>
       <c r="H385" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="386">
@@ -12940,7 +12928,7 @@
         <v>93.72835162357421</v>
       </c>
       <c r="H396" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="397">
@@ -12992,7 +12980,7 @@
         <v>23.242576191962144</v>
       </c>
       <c r="H398" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="399">
@@ -13070,7 +13058,7 @@
         <v>27.115006642781168</v>
       </c>
       <c r="H401" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="402">
@@ -13096,7 +13084,7 @@
         <v>24.578036909926595</v>
       </c>
       <c r="H402" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="403">
@@ -13356,7 +13344,7 @@
         <v>29.05674840954373</v>
       </c>
       <c r="H412" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="413">
@@ -13382,7 +13370,7 @@
         <v>820.4662296044778</v>
       </c>
       <c r="H413" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="414">
@@ -13408,7 +13396,7 @@
         <v>975.7588740746849</v>
       </c>
       <c r="H414" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="415">
@@ -13434,7 +13422,7 @@
         <v>547.1639215248015</v>
       </c>
       <c r="H415" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
     </row>
     <row r="416">
@@ -13460,7 +13448,7 @@
         <v>795.7036022549179</v>
       </c>
       <c r="H416" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="417">
@@ -13486,7 +13474,7 @@
         <v>1013.3294537173252</v>
       </c>
       <c r="H417" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="418">
@@ -13512,7 +13500,7 @@
         <v>602.1564159709178</v>
       </c>
       <c r="H418" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
     </row>
     <row r="419">
@@ -13538,7 +13526,7 @@
         <v>1349.0357438800552</v>
       </c>
       <c r="H419" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="420">
@@ -13564,7 +13552,7 @@
         <v>1374.9872528937399</v>
       </c>
       <c r="H420" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="421">
@@ -13590,7 +13578,7 @@
         <v>814.8849119915251</v>
       </c>
       <c r="H421" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="422">
@@ -13616,7 +13604,7 @@
         <v>968.0809884555902</v>
       </c>
       <c r="H422" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="423">
@@ -13642,7 +13630,7 @@
         <v>608.4556033736792</v>
       </c>
       <c r="H423" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="424">
@@ -13668,7 +13656,7 @@
         <v>764.2991737781049</v>
       </c>
       <c r="H424" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="425">
@@ -13694,7 +13682,7 @@
         <v>542.7951718783276</v>
       </c>
       <c r="H425" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
     </row>
     <row r="426">
@@ -13720,7 +13708,7 @@
         <v>677.8357128185826</v>
       </c>
       <c r="H426" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="427">
@@ -13746,7 +13734,7 @@
         <v>577.5127467136359</v>
       </c>
       <c r="H427" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
     </row>
     <row r="428">
@@ -13772,7 +13760,7 @@
         <v>1145.6177896008535</v>
       </c>
       <c r="H428" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="429">
@@ -13798,7 +13786,7 @@
         <v>900.0463888077819</v>
       </c>
       <c r="H429" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="430">
@@ -13824,7 +13812,7 @@
         <v>660.4358463374238</v>
       </c>
       <c r="H430" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="431">
@@ -13850,7 +13838,7 @@
         <v>48.936804308555224</v>
       </c>
       <c r="H431" t="s">
-        <v>589</v>
+        <v>583</v>
       </c>
     </row>
     <row r="432">
@@ -13876,7 +13864,7 @@
         <v>48.8460274914853</v>
       </c>
       <c r="H432" t="s">
-        <v>589</v>
+        <v>583</v>
       </c>
     </row>
     <row r="433">
@@ -13902,7 +13890,7 @@
         <v>48.81121319311205</v>
       </c>
       <c r="H433" t="s">
-        <v>589</v>
+        <v>583</v>
       </c>
     </row>
     <row r="434">
@@ -13928,7 +13916,7 @@
         <v>48.06152509610126</v>
       </c>
       <c r="H434" t="s">
-        <v>589</v>
+        <v>583</v>
       </c>
     </row>
     <row r="435">
@@ -13954,7 +13942,7 @@
         <v>47.81411551323629</v>
       </c>
       <c r="H435" t="s">
-        <v>589</v>
+        <v>583</v>
       </c>
     </row>
     <row r="436">
@@ -13980,7 +13968,7 @@
         <v>51.42532687836149</v>
       </c>
       <c r="H436" t="s">
-        <v>589</v>
+        <v>583</v>
       </c>
     </row>
     <row r="437">
@@ -14006,7 +13994,7 @@
         <v>48.1021936861157</v>
       </c>
       <c r="H437" t="s">
-        <v>590</v>
+        <v>584</v>
       </c>
     </row>
     <row r="438">
@@ -14032,7 +14020,7 @@
         <v>45.558154195753445</v>
       </c>
       <c r="H438" t="s">
-        <v>590</v>
+        <v>584</v>
       </c>
     </row>
     <row r="439">
@@ -14058,7 +14046,7 @@
         <v>48.030862200194406</v>
       </c>
       <c r="H439" t="s">
-        <v>590</v>
+        <v>584</v>
       </c>
     </row>
     <row r="440">
@@ -14084,7 +14072,7 @@
         <v>49.75536422236314</v>
       </c>
       <c r="H440" t="s">
-        <v>589</v>
+        <v>583</v>
       </c>
     </row>
     <row r="441">
@@ -14110,7 +14098,7 @@
         <v>48.20412223315145</v>
       </c>
       <c r="H441" t="s">
-        <v>589</v>
+        <v>583</v>
       </c>
     </row>
     <row r="442">
@@ -14136,7 +14124,7 @@
         <v>44.58786117828379</v>
       </c>
       <c r="H442" t="s">
-        <v>590</v>
+        <v>584</v>
       </c>
     </row>
     <row r="443">
@@ -14162,7 +14150,7 @@
         <v>46.94745340662621</v>
       </c>
       <c r="H443" t="s">
-        <v>589</v>
+        <v>583</v>
       </c>
     </row>
     <row r="444">
@@ -14188,7 +14176,7 @@
         <v>61.495307111460534</v>
       </c>
       <c r="H444" t="s">
-        <v>589</v>
+        <v>583</v>
       </c>
     </row>
     <row r="445">
@@ -14214,7 +14202,7 @@
         <v>55.609910859529236</v>
       </c>
       <c r="H445" t="s">
-        <v>589</v>
+        <v>583</v>
       </c>
     </row>
     <row r="446">
@@ -14240,7 +14228,7 @@
         <v>50.98812226453947</v>
       </c>
       <c r="H446" t="s">
-        <v>589</v>
+        <v>583</v>
       </c>
     </row>
     <row r="447">
@@ -14266,7 +14254,7 @@
         <v>50.584680153113254</v>
       </c>
       <c r="H447" t="s">
-        <v>589</v>
+        <v>583</v>
       </c>
     </row>
     <row r="448">
@@ -14292,7 +14280,7 @@
         <v>76.5111380644471</v>
       </c>
       <c r="H448" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="449">
@@ -14318,7 +14306,7 @@
         <v>73.27955247540092</v>
       </c>
       <c r="H449" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="450">
@@ -14344,7 +14332,7 @@
         <v>74.23385433637065</v>
       </c>
       <c r="H450" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="451">
@@ -14370,7 +14358,7 @@
         <v>75.30378381722983</v>
       </c>
       <c r="H451" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="452">
@@ -14396,7 +14384,7 @@
         <v>68.29272227891909</v>
       </c>
       <c r="H452" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="453">
@@ -14422,7 +14410,7 @@
         <v>62.698527899722194</v>
       </c>
       <c r="H453" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="454">
@@ -14448,7 +14436,7 @@
         <v>54.41310096437962</v>
       </c>
       <c r="H454" t="s">
-        <v>590</v>
+        <v>584</v>
       </c>
     </row>
     <row r="455">
@@ -14474,7 +14462,7 @@
         <v>81.82607562485157</v>
       </c>
       <c r="H455" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="456">
@@ -14526,7 +14514,7 @@
         <v>49.98355042363994</v>
       </c>
       <c r="H457" t="s">
-        <v>589</v>
+        <v>583</v>
       </c>
     </row>
     <row r="458">
@@ -14552,7 +14540,7 @@
         <v>88.15441831748853</v>
       </c>
       <c r="H458" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="459">
@@ -14578,7 +14566,7 @@
         <v>61.806000859446044</v>
       </c>
       <c r="H459" t="s">
-        <v>589</v>
+        <v>583</v>
       </c>
     </row>
     <row r="460">
@@ -14604,7 +14592,7 @@
         <v>53.79590505450483</v>
       </c>
       <c r="H460" t="s">
-        <v>589</v>
+        <v>583</v>
       </c>
     </row>
     <row r="461">
@@ -14630,7 +14618,7 @@
         <v>49.82807619456753</v>
       </c>
       <c r="H461" t="s">
-        <v>589</v>
+        <v>583</v>
       </c>
     </row>
     <row r="462">
@@ -14656,7 +14644,7 @@
         <v>63.09378194750104</v>
       </c>
       <c r="H462" t="s">
-        <v>589</v>
+        <v>583</v>
       </c>
     </row>
     <row r="463">
@@ -14682,7 +14670,7 @@
         <v>55.8409227511429</v>
       </c>
       <c r="H463" t="s">
-        <v>589</v>
+        <v>583</v>
       </c>
     </row>
     <row r="464">
@@ -14708,7 +14696,7 @@
         <v>104.33366539663825</v>
       </c>
       <c r="H464" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="465">
@@ -14734,7 +14722,7 @@
         <v>111.66851557308007</v>
       </c>
       <c r="H465" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="466">
@@ -14760,7 +14748,7 @@
         <v>95.58764176974546</v>
       </c>
       <c r="H466" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="467">
@@ -14786,7 +14774,7 @@
         <v>98.70339862012179</v>
       </c>
       <c r="H467" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="468">
@@ -14812,7 +14800,7 @@
         <v>68.4157788883798</v>
       </c>
       <c r="H468" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="469">
@@ -14838,7 +14826,7 @@
         <v>106.44936375650968</v>
       </c>
       <c r="H469" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="470">
@@ -14864,7 +14852,7 @@
         <v>107.5320726372131</v>
       </c>
       <c r="H470" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="471">
@@ -14890,7 +14878,7 @@
         <v>93.1508956008621</v>
       </c>
       <c r="H471" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="472">
@@ -14916,7 +14904,7 @@
         <v>91.33237182534492</v>
       </c>
       <c r="H472" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="473">
@@ -14942,7 +14930,7 @@
         <v>92.10529196126595</v>
       </c>
       <c r="H473" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="474">
@@ -14968,7 +14956,7 @@
         <v>91.21595450410734</v>
       </c>
       <c r="H474" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="475">
@@ -14994,7 +14982,7 @@
         <v>87.77698675193517</v>
       </c>
       <c r="H475" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="476">
@@ -15020,7 +15008,7 @@
         <v>90.35115345092902</v>
       </c>
       <c r="H476" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="477">
@@ -15046,7 +15034,7 @@
         <v>88.34447938499943</v>
       </c>
       <c r="H477" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="478">
@@ -15072,7 +15060,7 @@
         <v>102.21117471703349</v>
       </c>
       <c r="H478" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="479">
@@ -15098,7 +15086,7 @@
         <v>92.95085813536537</v>
       </c>
       <c r="H479" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="480">
@@ -15124,7 +15112,7 @@
         <v>70.97316611469603</v>
       </c>
       <c r="H480" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="481">
@@ -15150,7 +15138,7 @@
         <v>135.9612020386951</v>
       </c>
       <c r="H481" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="482">
@@ -15176,7 +15164,7 @@
         <v>94.06843560594064</v>
       </c>
       <c r="H482" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="483">
@@ -15202,7 +15190,7 @@
         <v>442.8932808641961</v>
       </c>
       <c r="H483" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="484">
@@ -15228,7 +15216,7 @@
         <v>77.57837208477122</v>
       </c>
       <c r="H484" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="485">
@@ -15254,7 +15242,7 @@
         <v>197.98549352909208</v>
       </c>
       <c r="H485" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="486">
@@ -15280,7 +15268,7 @@
         <v>284.2788203563256</v>
       </c>
       <c r="H486" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="487">
@@ -15306,7 +15294,7 @@
         <v>10.394609966720395</v>
       </c>
       <c r="H487" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="488">
@@ -15332,7 +15320,7 @@
         <v>12.131217946999868</v>
       </c>
       <c r="H488" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="489">
@@ -15384,7 +15372,7 @@
         <v>16.28227771744116</v>
       </c>
       <c r="H490" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="491">
@@ -15410,7 +15398,7 @@
         <v>12.48283182022908</v>
       </c>
       <c r="H491" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="492">
@@ -15436,7 +15424,7 @@
         <v>9.736042130795568</v>
       </c>
       <c r="H492" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="493">
@@ -15462,7 +15450,7 @@
         <v>12.764632247981126</v>
       </c>
       <c r="H493" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="494">
@@ -15514,7 +15502,7 @@
         <v>12.11382826172337</v>
       </c>
       <c r="H495" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="496">
@@ -15540,7 +15528,7 @@
         <v>10.12494498229114</v>
       </c>
       <c r="H496" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="497">
@@ -15592,7 +15580,7 @@
         <v>13.44041010372382</v>
       </c>
       <c r="H498" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="499">
@@ -15644,7 +15632,7 @@
         <v>9.76849633911479</v>
       </c>
       <c r="H500" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="501">
@@ -15670,7 +15658,7 @@
         <v>10.008157677550798</v>
       </c>
       <c r="H501" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="502">
@@ -15696,7 +15684,7 @@
         <v>75.6581622322442</v>
       </c>
       <c r="H502" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="503">
@@ -15722,7 +15710,7 @@
         <v>18.304001992778694</v>
       </c>
       <c r="H503" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="504">
@@ -15748,7 +15736,7 @@
         <v>11.677386727944736</v>
       </c>
       <c r="H504" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="505">
@@ -15930,7 +15918,7 @@
         <v>24.833435934392128</v>
       </c>
       <c r="H511" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="512">
@@ -15956,7 +15944,7 @@
         <v>17.022166759629613</v>
       </c>
       <c r="H512" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="513">
@@ -15982,7 +15970,7 @@
         <v>219.9791800316649</v>
       </c>
       <c r="H513" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
     </row>
     <row r="514">
@@ -16008,7 +15996,7 @@
         <v>228.1325598817241</v>
       </c>
       <c r="H514" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
     </row>
     <row r="515">
@@ -16034,7 +16022,7 @@
         <v>219.57642642166468</v>
       </c>
       <c r="H515" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
     </row>
     <row r="516">
@@ -16060,7 +16048,7 @@
         <v>219.4795388517972</v>
       </c>
       <c r="H516" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
     </row>
     <row r="517">
@@ -16086,7 +16074,7 @@
         <v>223.3136102182658</v>
       </c>
       <c r="H517" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
     </row>
     <row r="518">
@@ -16112,7 +16100,7 @@
         <v>228.74127917501812</v>
       </c>
       <c r="H518" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
     </row>
     <row r="519">
@@ -16138,7 +16126,7 @@
         <v>264.5797275636006</v>
       </c>
       <c r="H519" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
     </row>
     <row r="520">
@@ -16164,7 +16152,7 @@
         <v>221.76742696812016</v>
       </c>
       <c r="H520" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
     </row>
     <row r="521">
@@ -16190,7 +16178,7 @@
         <v>220.4146650663588</v>
       </c>
       <c r="H521" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
     </row>
     <row r="522">
@@ -16216,7 +16204,7 @@
         <v>218.39041627616848</v>
       </c>
       <c r="H522" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
     </row>
     <row r="523">
@@ -16242,7 +16230,7 @@
         <v>218.19350125299377</v>
       </c>
       <c r="H523" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
     </row>
     <row r="524">
@@ -16268,7 +16256,7 @@
         <v>252.10891742914555</v>
       </c>
       <c r="H524" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="525">
@@ -16294,7 +16282,7 @@
         <v>279.30862774276363</v>
       </c>
       <c r="H525" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="526">
@@ -16320,7 +16308,7 @@
         <v>159.85713149760136</v>
       </c>
       <c r="H526" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="527">
@@ -16346,7 +16334,7 @@
         <v>206.76055744874884</v>
       </c>
       <c r="H527" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="528">
@@ -16372,7 +16360,7 @@
         <v>185.21340838451124</v>
       </c>
       <c r="H528" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="529">
@@ -16398,7 +16386,7 @@
         <v>332.45591095826705</v>
       </c>
       <c r="H529" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="530">
@@ -16424,7 +16412,7 @@
         <v>157.0846240429354</v>
       </c>
       <c r="H530" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="531">
@@ -16450,7 +16438,7 @@
         <v>288.2122849560576</v>
       </c>
       <c r="H531" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="532">
@@ -16476,7 +16464,7 @@
         <v>137.68674565346896</v>
       </c>
       <c r="H532" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="533">
@@ -16502,7 +16490,7 @@
         <v>95.43729323190485</v>
       </c>
       <c r="H533" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="534">
@@ -16528,7 +16516,7 @@
         <v>91.86485310683872</v>
       </c>
       <c r="H534" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="535">
@@ -16554,7 +16542,7 @@
         <v>128.79334558088078</v>
       </c>
       <c r="H535" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="536">
@@ -16580,7 +16568,7 @@
         <v>173.77254081099147</v>
       </c>
       <c r="H536" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="537">
@@ -16606,7 +16594,7 @@
         <v>179.002212492255</v>
       </c>
       <c r="H537" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="538">
@@ -16632,7 +16620,7 @@
         <v>175.3386987911233</v>
       </c>
       <c r="H538" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="539">
@@ -16658,7 +16646,7 @@
         <v>179.11852998478344</v>
       </c>
       <c r="H539" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="540">
@@ -16684,7 +16672,7 @@
         <v>180.65551237432237</v>
       </c>
       <c r="H540" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="541">
@@ -16710,7 +16698,7 @@
         <v>181.66110585354477</v>
       </c>
       <c r="H541" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="542">
@@ -16736,7 +16724,7 @@
         <v>182.18734629608957</v>
       </c>
       <c r="H542" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="543">
@@ -16762,7 +16750,7 @@
         <v>223.69145844805394</v>
       </c>
       <c r="H543" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="544">
@@ -16788,7 +16776,7 @@
         <v>149.71120207015292</v>
       </c>
       <c r="H544" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
     </row>
     <row r="545">
@@ -16814,7 +16802,7 @@
         <v>153.2220122682496</v>
       </c>
       <c r="H545" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
     </row>
     <row r="546">
@@ -16840,7 +16828,7 @@
         <v>173.04099107042555</v>
       </c>
       <c r="H546" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="547">
@@ -16866,7 +16854,7 @@
         <v>150.2985180817759</v>
       </c>
       <c r="H547" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#1 update iTRAQI index cut points
</commit_message>
<xml_diff>
--- a/output/download-data/iTRAQI - ASGS 2021 SA2.xlsx
+++ b/output/download-data/iTRAQI - ASGS 2021 SA2.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1123" uniqueCount="588">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1123" uniqueCount="587">
   <si>
     <t>Suggested citation</t>
   </si>
@@ -1794,9 +1794,6 @@
   </si>
   <si>
     <t>5C</t>
-  </si>
-  <si>
-    <t>6C</t>
   </si>
   <si>
     <t>5B</t>
@@ -8118,7 +8115,7 @@
         <v>444.01763271334164</v>
       </c>
       <c r="H211" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="212">
@@ -8170,7 +8167,7 @@
         <v>428.7984201950769</v>
       </c>
       <c r="H213" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="214">
@@ -15970,7 +15967,7 @@
         <v>219.9791800316649</v>
       </c>
       <c r="H513" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="514">
@@ -15996,7 +15993,7 @@
         <v>228.1325598817241</v>
       </c>
       <c r="H514" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="515">
@@ -16022,7 +16019,7 @@
         <v>219.57642642166468</v>
       </c>
       <c r="H515" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="516">
@@ -16048,7 +16045,7 @@
         <v>219.4795388517972</v>
       </c>
       <c r="H516" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="517">
@@ -16074,7 +16071,7 @@
         <v>223.3136102182658</v>
       </c>
       <c r="H517" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="518">
@@ -16100,7 +16097,7 @@
         <v>228.74127917501812</v>
       </c>
       <c r="H518" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="519">
@@ -16126,7 +16123,7 @@
         <v>264.5797275636006</v>
       </c>
       <c r="H519" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="520">
@@ -16152,7 +16149,7 @@
         <v>221.76742696812016</v>
       </c>
       <c r="H520" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="521">
@@ -16178,7 +16175,7 @@
         <v>220.4146650663588</v>
       </c>
       <c r="H521" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="522">
@@ -16204,7 +16201,7 @@
         <v>218.39041627616848</v>
       </c>
       <c r="H522" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="523">
@@ -16230,7 +16227,7 @@
         <v>218.19350125299377</v>
       </c>
       <c r="H523" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="524">
@@ -16776,7 +16773,7 @@
         <v>149.71120207015292</v>
       </c>
       <c r="H544" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="545">
@@ -16802,7 +16799,7 @@
         <v>153.2220122682496</v>
       </c>
       <c r="H545" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="546">
@@ -16854,7 +16851,7 @@
         <v>150.2985180817759</v>
       </c>
       <c r="H547" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
   </sheetData>

</xml_diff>